<commit_message>
updated Original Drug List xlsx
Some are still missing, including those -mab and filgrastim, which have several entries on PubChem, and I don't know which to use.
</commit_message>
<xml_diff>
--- a/Breast Drug List.xlsx
+++ b/Breast Drug List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mycuhk-my.sharepoint.com/personal/1155143802_link_cuhk_edu_hk/Documents/GitHub/Pharmacy Automation - Breast Cancer HDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8630272-EE4D-4884-A84E-3D54AE849AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{F8630272-EE4D-4884-A84E-3D54AE849AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{820761AF-FA37-0B45-8515-63A9790D86C8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{73AACD8B-5989-4315-B966-A20FBBA35E6F}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{73AACD8B-5989-4315-B966-A20FBBA35E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,15 +50,9 @@
     <t>Epirubicin</t>
   </si>
   <si>
-    <t>5-Fluoruouracil</t>
-  </si>
-  <si>
     <t>Docetaxel</t>
   </si>
   <si>
-    <t>Palictaxel</t>
-  </si>
-  <si>
     <t>Carboplatin</t>
   </si>
   <si>
@@ -74,24 +68,15 @@
     <t>Adjunctive treatment</t>
   </si>
   <si>
-    <t>Akynzeo</t>
-  </si>
-  <si>
     <t>Emend</t>
   </si>
   <si>
     <t>Filgrastim</t>
   </si>
   <si>
-    <t>Metochlorpamide</t>
-  </si>
-  <si>
     <t>Loperamide</t>
   </si>
   <si>
-    <t>Thymol gargle</t>
-  </si>
-  <si>
     <t>Eribulin</t>
   </si>
   <si>
@@ -183,6 +168,21 @@
   </si>
   <si>
     <t>Nab-paclitaxel</t>
+  </si>
+  <si>
+    <t>5-Fluorouracil</t>
+  </si>
+  <si>
+    <t>Paclitaxel</t>
+  </si>
+  <si>
+    <t>Thymol</t>
+  </si>
+  <si>
+    <t>Metoclopramide</t>
+  </si>
+  <si>
+    <t>Netupitant mixture with palonosetron</t>
   </si>
 </sst>
 </file>
@@ -244,6 +244,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE7F14C-5175-4DA6-A68F-5446C16B20A3}">
   <dimension ref="A2:A72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,227 +577,227 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>